<commit_message>
Update data and export to .sql
</commit_message>
<xml_diff>
--- a/Documentation/prototype_data_base_donnees.xlsx
+++ b/Documentation/prototype_data_base_donnees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpnv\projProg\CargoFlow\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C825ADA-6544-4102-9D97-BD4B6545FC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1E6BCB-0636-4943-A9E7-6CF7F571DDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03DA1F0F-3B6E-41FA-B428-2227A02C2D02}"/>
   </bookViews>
@@ -579,33 +579,18 @@
     <t>2023-02-15 10:00:00</t>
   </si>
   <si>
-    <t>2023-02-15 14:30:00</t>
-  </si>
-  <si>
     <t>2023-02-16 08:45:00</t>
   </si>
   <si>
-    <t>2023-02-16 11:15:00</t>
-  </si>
-  <si>
     <t>2023-02-17 14:20:00</t>
   </si>
   <si>
-    <t>2023-02-17 18:45:00</t>
-  </si>
-  <si>
     <t>2023-02-18 11:30:00</t>
   </si>
   <si>
-    <t>2023-02-18 16:00:00</t>
-  </si>
-  <si>
     <t>2023-02-19 09:15:00</t>
   </si>
   <si>
-    <t>2023-02-19 12:45:00</t>
-  </si>
-  <si>
     <t>0041581234567</t>
   </si>
   <si>
@@ -619,6 +604,21 @@
   </si>
   <si>
     <t>0041911234567</t>
+  </si>
+  <si>
+    <t>2023-02-18 14:30:00</t>
+  </si>
+  <si>
+    <t>2023-02-17 11:15:00</t>
+  </si>
+  <si>
+    <t>2023-02-18 18:45:00</t>
+  </si>
+  <si>
+    <t>2023-03-01 16:00:00</t>
+  </si>
+  <si>
+    <t>2023-02-26 12:45:00</t>
   </si>
 </sst>
 </file>
@@ -1069,6 +1069,10 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,10 +1082,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1413,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0A263E-AF56-467B-8C8D-FA9E6A0C67C4}">
   <dimension ref="B2:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K38" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="C72" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1437,18 +1437,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="2:13">
       <c r="B3" s="1" t="s">
@@ -1513,7 +1513,7 @@
       <c r="K4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="73" t="str">
+      <c r="M4" s="70" t="str">
         <f>"INSERT INTO " &amp; articles &amp; " (" &amp; C$3 &amp; "," &amp; D$3 &amp; "," &amp; E$3 &amp; "," &amp; F$3 &amp; "," &amp; G$3 &amp; "," &amp; H$3 &amp; "," &amp; I$3 &amp; "," &amp; J$3 &amp; "," &amp; K$3 &amp; ") VALUES ('" &amp; C4 &amp; "','" &amp; D4 &amp; "','" &amp; E4 &amp; "','" &amp; F4 &amp; "','" &amp; G4 &amp; "','" &amp; H4 &amp; "','" &amp; I4 &amp; "','" &amp; J4 &amp; "','" &amp; K4 &amp; "')"</f>
         <v>INSERT INTO articles (barcode,model,brand,weight,height,lenght,width,price,category_id) VALUES ('123456789012','Galaxy S21','Samsung','0.2','15','7.5','0.8','1099.9','1')</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="K5" s="4">
         <v>2</v>
       </c>
-      <c r="M5" s="73" t="str">
+      <c r="M5" s="70" t="str">
         <f>"INSERT INTO " &amp; articles &amp; " (" &amp; C$3 &amp; "," &amp; D$3 &amp; "," &amp; E$3 &amp; "," &amp; F$3 &amp; "," &amp; G$3 &amp; "," &amp; H$3 &amp; "," &amp; I$3 &amp; "," &amp; J$3 &amp; "," &amp; K$3 &amp; ") VALUES ('" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "','" &amp; F5 &amp; "','" &amp; G5 &amp; "','" &amp; H5 &amp; "','" &amp; I5 &amp; "','" &amp; J5 &amp; "','" &amp; K5 &amp; "')"</f>
         <v>INSERT INTO articles (barcode,model,brand,weight,height,lenght,width,price,category_id) VALUES ('987654321098','Slim Fit Jeans','Levi's','0.7','110','50','0.5','79.9','2')</v>
       </c>
@@ -1585,7 +1585,7 @@
       <c r="K6" s="4">
         <v>3</v>
       </c>
-      <c r="M6" s="73" t="str">
+      <c r="M6" s="70" t="str">
         <f>"INSERT INTO " &amp; articles &amp; " (" &amp; C$3 &amp; "," &amp; D$3 &amp; "," &amp; E$3 &amp; "," &amp; F$3 &amp; "," &amp; G$3 &amp; "," &amp; H$3 &amp; "," &amp; I$3 &amp; "," &amp; J$3 &amp; "," &amp; K$3 &amp; ") VALUES ('" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "','" &amp; F6 &amp; "','" &amp; G6 &amp; "','" &amp; H6 &amp; "','" &amp; I6 &amp; "','" &amp; J6 &amp; "','" &amp; K6 &amp; "')"</f>
         <v>INSERT INTO articles (barcode,model,brand,weight,height,lenght,width,price,category_id) VALUES ('567890123456','Ektorp Sofa','IKEA','25','80','200','100','999.9','3')</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="K7" s="4">
         <v>4</v>
       </c>
-      <c r="M7" s="73" t="str">
+      <c r="M7" s="70" t="str">
         <f>"INSERT INTO " &amp; articles &amp; " (" &amp; C$3 &amp; "," &amp; D$3 &amp; "," &amp; E$3 &amp; "," &amp; F$3 &amp; "," &amp; G$3 &amp; "," &amp; H$3 &amp; "," &amp; I$3 &amp; "," &amp; J$3 &amp; "," &amp; K$3 &amp; ") VALUES ('" &amp; C7 &amp; "','" &amp; D7 &amp; "','" &amp; E7 &amp; "','" &amp; F7 &amp; "','" &amp; G7 &amp; "','" &amp; H7 &amp; "','" &amp; I7 &amp; "','" &amp; J7 &amp; "','" &amp; K7 &amp; "')"</f>
         <v>INSERT INTO articles (barcode,model,brand,weight,height,lenght,width,price,category_id) VALUES ('345678901234','Air Zoom Pegasus','Nike','0.5','12','30','10','129.9','4')</v>
       </c>
@@ -1657,19 +1657,19 @@
       <c r="K8" s="4">
         <v>5</v>
       </c>
-      <c r="M8" s="73" t="str">
+      <c r="M8" s="70" t="str">
         <f>"INSERT INTO " &amp; articles &amp; " (" &amp; C$3 &amp; "," &amp; D$3 &amp; "," &amp; E$3 &amp; "," &amp; F$3 &amp; "," &amp; G$3 &amp; "," &amp; H$3 &amp; "," &amp; I$3 &amp; "," &amp; J$3 &amp; "," &amp; K$3 &amp; ") VALUES ('" &amp; C8 &amp; "','" &amp; D8 &amp; "','" &amp; E8 &amp; "','" &amp; F8 &amp; "','" &amp; G8 &amp; "','" &amp; H8 &amp; "','" &amp; I8 &amp; "','" &amp; J8 &amp; "','" &amp; K8 &amp; "')"</f>
         <v>INSERT INTO articles (barcode,model,brand,weight,height,lenght,width,price,category_id) VALUES ('789012345678','Kindle Oasis','Amazon','0.3','20','15','1','199.9','5')</v>
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="1" t="s">
@@ -1702,7 +1702,7 @@
         <v>45</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M12" s="1" t="str">
         <f>"INSERT INTO " &amp; carriers &amp; " (" &amp; C$11&amp; "," &amp; D$11 &amp; "," &amp; E$11 &amp; "," &amp; F$11 &amp; ") VALUES ('" &amp; C12 &amp; "','" &amp; D12 &amp; "','" &amp; E12 &amp; "','" &amp; F12 &amp; "')"</f>
@@ -1723,7 +1723,7 @@
         <v>46</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="M13" s="1" t="str">
         <f>"INSERT INTO " &amp; carriers &amp; " (" &amp; C$11&amp; "," &amp; D$11 &amp; "," &amp; E$11 &amp; "," &amp; F$11 &amp; ") VALUES ('" &amp; C13 &amp; "','" &amp; D13 &amp; "','" &amp; E13 &amp; "','" &amp; F13 &amp; "')"</f>
@@ -1744,7 +1744,7 @@
         <v>47</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M14" s="1" t="str">
         <f>"INSERT INTO " &amp; carriers &amp; " (" &amp; C$11&amp; "," &amp; D$11 &amp; "," &amp; E$11 &amp; "," &amp; F$11 &amp; ") VALUES ('" &amp; C14 &amp; "','" &amp; D14 &amp; "','" &amp; E14 &amp; "','" &amp; F14 &amp; "')"</f>
@@ -1765,7 +1765,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="64" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="M15" s="1" t="str">
         <f>"INSERT INTO " &amp; carriers &amp; " (" &amp; C$11&amp; "," &amp; D$11 &amp; "," &amp; E$11 &amp; "," &amp; F$11 &amp; ") VALUES ('" &amp; C15 &amp; "','" &amp; D15 &amp; "','" &amp; E15 &amp; "','" &amp; F15 &amp; "')"</f>
@@ -1786,7 +1786,7 @@
         <v>49</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M16" s="1" t="str">
         <f>"INSERT INTO " &amp; carriers &amp; " (" &amp; C$11&amp; "," &amp; D$11 &amp; "," &amp; E$11 &amp; "," &amp; F$11 &amp; ") VALUES ('" &amp; C16 &amp; "','" &amp; D16 &amp; "','" &amp; E16 &amp; "','" &amp; F16 &amp; "')"</f>
@@ -1794,11 +1794,11 @@
       </c>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="74"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="1" t="s">
@@ -1887,16 +1887,16 @@
       </c>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="72"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="74"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="1" t="s">
@@ -1934,7 +1934,7 @@
       <c r="D28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="71" t="s">
         <v>105</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1964,7 +1964,7 @@
       <c r="D29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="71" t="s">
         <v>106</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1994,7 +1994,7 @@
       <c r="D30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="74" t="s">
+      <c r="E30" s="71" t="s">
         <v>107</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -2024,7 +2024,7 @@
       <c r="D31" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="74" t="s">
+      <c r="E31" s="71" t="s">
         <v>108</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -2054,7 +2054,7 @@
       <c r="D32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="74" t="s">
+      <c r="E32" s="71" t="s">
         <v>104</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -2075,10 +2075,10 @@
       </c>
     </row>
     <row r="34" spans="2:17">
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="72"/>
+      <c r="C34" s="74"/>
     </row>
     <row r="35" spans="2:17">
       <c r="B35" s="1" t="s">
@@ -2149,17 +2149,17 @@
       </c>
     </row>
     <row r="42" spans="2:17">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="72"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="74"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -2208,7 +2208,7 @@
         <v>175</v>
       </c>
       <c r="E44" s="64" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>35</v>
@@ -2225,9 +2225,9 @@
       <c r="J44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M44" s="73" t="str">
+      <c r="M44" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries &amp; " (" &amp; C$43 &amp; "," &amp; D$43 &amp; "," &amp; E$43 &amp; "," &amp; F$43 &amp; "," &amp; G$43 &amp; "," &amp; H$43 &amp; "," &amp; I$43 &amp; "," &amp; J$43 &amp; ") VALUES ('" &amp; C44 &amp; "','" &amp; D44 &amp; "','" &amp; E44 &amp; "','" &amp; F44 &amp; "','" &amp; G44 &amp; "','" &amp; H44 &amp; "','" &amp; I44 &amp; "','" &amp; J44 &amp; "')"</f>
-        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('123456789012','2023-02-15 10:00:00','2023-02-15 14:30:00','Livré','1','1','1','null')</v>
+        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('123456789012','2023-02-15 10:00:00','2023-02-18 14:30:00','Livré','1','1','1','null')</v>
       </c>
     </row>
     <row r="45" spans="2:17">
@@ -2238,10 +2238,10 @@
         <v>987654321098</v>
       </c>
       <c r="D45" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E45" s="64" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>36</v>
@@ -2258,9 +2258,9 @@
       <c r="J45" s="51">
         <v>3</v>
       </c>
-      <c r="M45" s="73" t="str">
+      <c r="M45" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries &amp; " (" &amp; C$43 &amp; "," &amp; D$43 &amp; "," &amp; E$43 &amp; "," &amp; F$43 &amp; "," &amp; G$43 &amp; "," &amp; H$43 &amp; "," &amp; I$43 &amp; "," &amp; J$43 &amp; ") VALUES ('" &amp; C45 &amp; "','" &amp; D45 &amp; "','" &amp; E45 &amp; "','" &amp; F45 &amp; "','" &amp; G45 &amp; "','" &amp; H45 &amp; "','" &amp; I45 &amp; "','" &amp; J45 &amp; "')"</f>
-        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('987654321098','2023-02-16 08:45:00','2023-02-16 11:15:00','En transit','2','null','2','3')</v>
+        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('987654321098','2023-02-16 08:45:00','2023-02-17 11:15:00','En transit','2','null','2','3')</v>
       </c>
     </row>
     <row r="46" spans="2:17">
@@ -2271,10 +2271,10 @@
         <v>567890123456</v>
       </c>
       <c r="D46" s="64" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E46" s="64" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>37</v>
@@ -2291,9 +2291,9 @@
       <c r="J46" s="53">
         <v>5</v>
       </c>
-      <c r="M46" s="73" t="str">
+      <c r="M46" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries &amp; " (" &amp; C$43 &amp; "," &amp; D$43 &amp; "," &amp; E$43 &amp; "," &amp; F$43 &amp; "," &amp; G$43 &amp; "," &amp; H$43 &amp; "," &amp; I$43 &amp; "," &amp; J$43 &amp; ") VALUES ('" &amp; C46 &amp; "','" &amp; D46 &amp; "','" &amp; E46 &amp; "','" &amp; F46 &amp; "','" &amp; G46 &amp; "','" &amp; H46 &amp; "','" &amp; I46 &amp; "','" &amp; J46 &amp; "')"</f>
-        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('567890123456','2023-02-17 14:20:00','2023-02-17 18:45:00','Planifié','3','null','3','5')</v>
+        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('567890123456','2023-02-17 14:20:00','2023-02-18 18:45:00','Planifié','3','null','3','5')</v>
       </c>
     </row>
     <row r="47" spans="2:17">
@@ -2304,10 +2304,10 @@
         <v>345678901234</v>
       </c>
       <c r="D47" s="64" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E47" s="64" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>36</v>
@@ -2324,9 +2324,9 @@
       <c r="J47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M47" s="73" t="str">
+      <c r="M47" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries &amp; " (" &amp; C$43 &amp; "," &amp; D$43 &amp; "," &amp; E$43 &amp; "," &amp; F$43 &amp; "," &amp; G$43 &amp; "," &amp; H$43 &amp; "," &amp; I$43 &amp; "," &amp; J$43 &amp; ") VALUES ('" &amp; C47 &amp; "','" &amp; D47 &amp; "','" &amp; E47 &amp; "','" &amp; F47 &amp; "','" &amp; G47 &amp; "','" &amp; H47 &amp; "','" &amp; I47 &amp; "','" &amp; J47 &amp; "')"</f>
-        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('345678901234','2023-02-18 11:30:00','2023-02-18 16:00:00','En transit','4','5','4','null')</v>
+        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('345678901234','2023-02-18 11:30:00','2023-03-01 16:00:00','En transit','4','5','4','null')</v>
       </c>
     </row>
     <row r="48" spans="2:17">
@@ -2337,10 +2337,10 @@
         <v>789012345678</v>
       </c>
       <c r="D48" s="64" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E48" s="64" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>35</v>
@@ -2357,18 +2357,18 @@
       <c r="J48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M48" s="73" t="str">
+      <c r="M48" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries &amp; " (" &amp; C$43 &amp; "," &amp; D$43 &amp; "," &amp; E$43 &amp; "," &amp; F$43 &amp; "," &amp; G$43 &amp; "," &amp; H$43 &amp; "," &amp; I$43 &amp; "," &amp; J$43 &amp; ") VALUES ('" &amp; C48 &amp; "','" &amp; D48 &amp; "','" &amp; E48 &amp; "','" &amp; F48 &amp; "','" &amp; G48 &amp; "','" &amp; H48 &amp; "','" &amp; I48 &amp; "','" &amp; J48 &amp; "')"</f>
-        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('789012345678','2023-02-19 09:15:00','2023-02-19 12:45:00','Livré','5','2','5','null')</v>
+        <v>INSERT INTO deliveries (barcode,startDate,endDate,status,carrier_id,client_id,warehouse_origin_id,warehouse_destination_id) VALUES ('789012345678','2023-02-19 09:15:00','2023-02-26 12:45:00','Livré','5','2','5','null')</v>
       </c>
     </row>
     <row r="50" spans="2:13">
-      <c r="B50" s="70" t="s">
+      <c r="B50" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="72"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="74"/>
     </row>
     <row r="51" spans="2:13">
       <c r="B51" s="1" t="s">
@@ -2397,7 +2397,7 @@
       <c r="E52" s="1">
         <v>32</v>
       </c>
-      <c r="M52" s="73" t="str">
+      <c r="M52" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries_have_articles &amp; " (" &amp; C$51 &amp; "," &amp; D$51 &amp; "," &amp; E$51 &amp; ") VALUES ('" &amp; C52 &amp; "','" &amp; D52 &amp; "','" &amp; E52 &amp; "')"</f>
         <v>INSERT INTO deliveries_have_articles (delivery_id,article_id,quantity) VALUES ('1','1','32')</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="E53" s="1">
         <v>15</v>
       </c>
-      <c r="M53" s="73" t="str">
+      <c r="M53" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries_have_articles &amp; " (" &amp; C$51 &amp; "," &amp; D$51 &amp; "," &amp; E$51 &amp; ") VALUES ('" &amp; C53 &amp; "','" &amp; D53 &amp; "','" &amp; E53 &amp; "')"</f>
         <v>INSERT INTO deliveries_have_articles (delivery_id,article_id,quantity) VALUES ('2','1','15')</v>
       </c>
@@ -2433,7 +2433,7 @@
       <c r="E54" s="1">
         <v>67</v>
       </c>
-      <c r="M54" s="73" t="str">
+      <c r="M54" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries_have_articles &amp; " (" &amp; C$51 &amp; "," &amp; D$51 &amp; "," &amp; E$51 &amp; ") VALUES ('" &amp; C54 &amp; "','" &amp; D54 &amp; "','" &amp; E54 &amp; "')"</f>
         <v>INSERT INTO deliveries_have_articles (delivery_id,article_id,quantity) VALUES ('3','2','67')</v>
       </c>
@@ -2451,7 +2451,7 @@
       <c r="E55" s="1">
         <v>36</v>
       </c>
-      <c r="M55" s="73" t="str">
+      <c r="M55" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries_have_articles &amp; " (" &amp; C$51 &amp; "," &amp; D$51 &amp; "," &amp; E$51 &amp; ") VALUES ('" &amp; C55 &amp; "','" &amp; D55 &amp; "','" &amp; E55 &amp; "')"</f>
         <v>INSERT INTO deliveries_have_articles (delivery_id,article_id,quantity) VALUES ('4','5','36')</v>
       </c>
@@ -2469,22 +2469,22 @@
       <c r="E56" s="1">
         <v>103</v>
       </c>
-      <c r="M56" s="73" t="str">
+      <c r="M56" s="70" t="str">
         <f>"INSERT INTO " &amp; deliveries_have_articles &amp; " (" &amp; C$51 &amp; "," &amp; D$51 &amp; "," &amp; E$51 &amp; ") VALUES ('" &amp; C56 &amp; "','" &amp; D56 &amp; "','" &amp; E56 &amp; "')"</f>
         <v>INSERT INTO deliveries_have_articles (delivery_id,article_id,quantity) VALUES ('5','5','103')</v>
       </c>
     </row>
     <row r="58" spans="2:13">
-      <c r="B58" s="70" t="s">
+      <c r="B58" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="71"/>
-      <c r="F58" s="71"/>
-      <c r="G58" s="71"/>
-      <c r="H58" s="71"/>
-      <c r="I58" s="72"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="74"/>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" s="1" t="s">
@@ -2525,7 +2525,7 @@
       <c r="E60" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F60" s="74" t="s">
+      <c r="F60" s="71" t="s">
         <v>133</v>
       </c>
       <c r="G60" s="64" t="s">
@@ -2537,7 +2537,7 @@
       <c r="I60" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M60" s="73" t="str">
+      <c r="M60" s="70" t="str">
         <f>"INSERT INTO " &amp; employees &amp; " (" &amp; C$59 &amp; "," &amp; D$59 &amp; "," &amp; E$59 &amp; "," &amp; F$59 &amp; "," &amp; G$59 &amp; "," &amp; H$59 &amp; "," &amp; I$59 &amp; "," &amp; J$59 &amp; ") VALUES ('" &amp; C60 &amp; "','" &amp; D60 &amp; "','" &amp; E60 &amp; "','" &amp; F60 &amp; "','" &amp; G60 &amp; "','" &amp; H60 &amp; "','" &amp; I60 &amp; "','" &amp; J60 &amp; "')"</f>
         <v>INSERT INTO employees (lastName,firstName,password,email,phoneNumber,role,employeeNumber,) VALUES ('Martin','Pierre','pmartin','pierre.martin@email.com','0041589876543','Gestionnaire','E1001','')</v>
       </c>
@@ -2555,7 +2555,7 @@
       <c r="E61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F61" s="74" t="s">
+      <c r="F61" s="71" t="s">
         <v>134</v>
       </c>
       <c r="G61" s="64" t="s">
@@ -2567,7 +2567,7 @@
       <c r="I61" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M61" s="73" t="str">
+      <c r="M61" s="70" t="str">
         <f>"INSERT INTO " &amp; employees &amp; " (" &amp; C$59 &amp; "," &amp; D$59 &amp; "," &amp; E$59 &amp; "," &amp; F$59 &amp; "," &amp; G$59 &amp; "," &amp; H$59 &amp; "," &amp; I$59 &amp; "," &amp; J$59 &amp; ") VALUES ('" &amp; C61 &amp; "','" &amp; D61 &amp; "','" &amp; E61 &amp; "','" &amp; F61 &amp; "','" &amp; G61 &amp; "','" &amp; H61 &amp; "','" &amp; I61 &amp; "','" &amp; J61 &amp; "')"</f>
         <v>INSERT INTO employees (lastName,firstName,password,email,phoneNumber,role,employeeNumber,) VALUES ('Favre','Marie','mfavre','marie.favre@email.com','0041249876543','Logistique','E1002','')</v>
       </c>
@@ -2585,7 +2585,7 @@
       <c r="E62" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F62" s="74" t="s">
+      <c r="F62" s="71" t="s">
         <v>135</v>
       </c>
       <c r="G62" s="64" t="s">
@@ -2597,7 +2597,7 @@
       <c r="I62" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M62" s="73" t="str">
+      <c r="M62" s="70" t="str">
         <f>"INSERT INTO " &amp; employees &amp; " (" &amp; C$59 &amp; "," &amp; D$59 &amp; "," &amp; E$59 &amp; "," &amp; F$59 &amp; "," &amp; G$59 &amp; "," &amp; H$59 &amp; "," &amp; I$59 &amp; "," &amp; J$59 &amp; ") VALUES ('" &amp; C62 &amp; "','" &amp; D62 &amp; "','" &amp; E62 &amp; "','" &amp; F62 &amp; "','" &amp; G62 &amp; "','" &amp; H62 &amp; "','" &amp; I62 &amp; "','" &amp; J62 &amp; "')"</f>
         <v>INSERT INTO employees (lastName,firstName,password,email,phoneNumber,role,employeeNumber,) VALUES ('Lefevre','Olivia','olefevre','olivia.lefevre@email.com','0041219876543','ServiceClient','E1003','')</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="E63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F63" s="74" t="s">
+      <c r="F63" s="71" t="s">
         <v>136</v>
       </c>
       <c r="G63" s="64" t="s">
@@ -2627,7 +2627,7 @@
       <c r="I63" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M63" s="73" t="str">
+      <c r="M63" s="70" t="str">
         <f>"INSERT INTO " &amp; employees &amp; " (" &amp; C$59 &amp; "," &amp; D$59 &amp; "," &amp; E$59 &amp; "," &amp; F$59 &amp; "," &amp; G$59 &amp; "," &amp; H$59 &amp; "," &amp; I$59 &amp; "," &amp; J$59 &amp; ") VALUES ('" &amp; C63 &amp; "','" &amp; D63 &amp; "','" &amp; E63 &amp; "','" &amp; F63 &amp; "','" &amp; G63 &amp; "','" &amp; H63 &amp; "','" &amp; I63 &amp; "','" &amp; J63 &amp; "')"</f>
         <v>INSERT INTO employees (lastName,firstName,password,email,phoneNumber,role,employeeNumber,) VALUES ('Leroux','Isabelle','ileroux','isabelle.leroux@email.com','0041229876543','Développeur','E1004','')</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="E64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F64" s="74" t="s">
+      <c r="F64" s="71" t="s">
         <v>137</v>
       </c>
       <c r="G64" s="64" t="s">
@@ -2657,20 +2657,20 @@
       <c r="I64" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M64" s="73" t="str">
+      <c r="M64" s="70" t="str">
         <f>"INSERT INTO " &amp; employees &amp; " (" &amp; C$59 &amp; "," &amp; D$59 &amp; "," &amp; E$59 &amp; "," &amp; F$59 &amp; "," &amp; G$59 &amp; "," &amp; H$59 &amp; "," &amp; I$59 &amp; "," &amp; J$59 &amp; ") VALUES ('" &amp; C64 &amp; "','" &amp; D64 &amp; "','" &amp; E64 &amp; "','" &amp; F64 &amp; "','" &amp; G64 &amp; "','" &amp; H64 &amp; "','" &amp; I64 &amp; "','" &amp; J64 &amp; "')"</f>
         <v>INSERT INTO employees (lastName,firstName,password,email,phoneNumber,role,employeeNumber,) VALUES ('Moreau','Nicolas','nmoreau','nicolas.moreau@email.com','0041919876543','Marketing','E1005','')</v>
       </c>
     </row>
     <row r="66" spans="2:13">
-      <c r="B66" s="70" t="s">
+      <c r="B66" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="71"/>
-      <c r="D66" s="71"/>
-      <c r="E66" s="71"/>
-      <c r="F66" s="71"/>
-      <c r="G66" s="72"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
+      <c r="F66" s="73"/>
+      <c r="G66" s="74"/>
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="2:13">
@@ -2712,7 +2712,7 @@
       <c r="G68" s="1">
         <v>75001</v>
       </c>
-      <c r="M68" s="73" t="str">
+      <c r="M68" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses &amp; " (" &amp; C$67 &amp; "," &amp; D$67 &amp; "," &amp; E$67 &amp; "," &amp; F$67 &amp; "," &amp; G$67 &amp; ") VALUES ('" &amp; C68 &amp; "','" &amp; D68 &amp; "','" &amp; E68 &amp; "','" &amp; F68 &amp; "','" &amp; G68 &amp; "')"</f>
         <v>INSERT INTO warehouses (name,street,streetNb,city,postalCode) VALUES ('StockExpress','Rue de la Logistique','22','Paris','75001')</v>
       </c>
@@ -2736,7 +2736,7 @@
       <c r="G69" s="1">
         <v>69002</v>
       </c>
-      <c r="M69" s="73" t="str">
+      <c r="M69" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses &amp; " (" &amp; C$67 &amp; "," &amp; D$67 &amp; "," &amp; E$67 &amp; "," &amp; F$67 &amp; "," &amp; G$67 &amp; ") VALUES ('" &amp; C69 &amp; "','" &amp; D69 &amp; "','" &amp; E69 &amp; "','" &amp; F69 &amp; "','" &amp; G69 &amp; "')"</f>
         <v>INSERT INTO warehouses (name,street,streetNb,city,postalCode) VALUES ('LogiStock','Avenue des Entrepôts','45','Lyon','69002')</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="G70" s="1">
         <v>20123</v>
       </c>
-      <c r="M70" s="73" t="str">
+      <c r="M70" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses &amp; " (" &amp; C$67 &amp; "," &amp; D$67 &amp; "," &amp; E$67 &amp; "," &amp; F$67 &amp; "," &amp; G$67 &amp; ") VALUES ('" &amp; C70 &amp; "','" &amp; D70 &amp; "','" &amp; E70 &amp; "','" &amp; F70 &amp; "','" &amp; G70 &amp; "')"</f>
         <v>INSERT INTO warehouses (name,street,streetNb,city,postalCode) VALUES ('MagazzinoItaliano','Via Magazzino','78','Milan','20123')</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="G71" s="1">
         <v>10115</v>
       </c>
-      <c r="M71" s="73" t="str">
+      <c r="M71" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses &amp; " (" &amp; C$67 &amp; "," &amp; D$67 &amp; "," &amp; E$67 &amp; "," &amp; F$67 &amp; "," &amp; G$67 &amp; ") VALUES ('" &amp; C71 &amp; "','" &amp; D71 &amp; "','" &amp; E71 &amp; "','" &amp; F71 &amp; "','" &amp; G71 &amp; "')"</f>
         <v>INSERT INTO warehouses (name,street,streetNb,city,postalCode) VALUES ('Lagerhaus','Am Lagerplatz','34','Berlin','10115')</v>
       </c>
@@ -2808,18 +2808,18 @@
       <c r="G72" s="1">
         <v>8001</v>
       </c>
-      <c r="M72" s="73" t="str">
+      <c r="M72" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses &amp; " (" &amp; C$67 &amp; "," &amp; D$67 &amp; "," &amp; E$67 &amp; "," &amp; F$67 &amp; "," &amp; G$67 &amp; ") VALUES ('" &amp; C72 &amp; "','" &amp; D72 &amp; "','" &amp; E72 &amp; "','" &amp; F72 &amp; "','" &amp; G72 &amp; "')"</f>
         <v>INSERT INTO warehouses (name,street,streetNb,city,postalCode) VALUES ('AlmacenCentral','Calle de Almacén','56','Barcelone','8001')</v>
       </c>
     </row>
     <row r="74" spans="2:13">
-      <c r="B74" s="70" t="s">
+      <c r="B74" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="C74" s="71"/>
-      <c r="D74" s="71"/>
-      <c r="E74" s="72"/>
+      <c r="C74" s="73"/>
+      <c r="D74" s="73"/>
+      <c r="E74" s="74"/>
     </row>
     <row r="75" spans="2:13">
       <c r="B75" s="1" t="s">
@@ -2848,7 +2848,7 @@
       <c r="E76" s="1">
         <v>6</v>
       </c>
-      <c r="M76" s="73" t="str">
+      <c r="M76" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_articles &amp; " (" &amp; C$75 &amp; "," &amp; D$75 &amp; "," &amp; E$75 &amp; ") VALUES ('" &amp; C76 &amp; "','" &amp; D76 &amp; "','" &amp; E76 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_articles (article_id,warehouse_id,quantity) VALUES ('1','2','6')</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="E77" s="1">
         <v>425</v>
       </c>
-      <c r="M77" s="73" t="str">
+      <c r="M77" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_articles &amp; " (" &amp; C$75 &amp; "," &amp; D$75 &amp; "," &amp; E$75 &amp; ") VALUES ('" &amp; C77 &amp; "','" &amp; D77 &amp; "','" &amp; E77 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_articles (article_id,warehouse_id,quantity) VALUES ('2','2','425')</v>
       </c>
@@ -2884,7 +2884,7 @@
       <c r="E78" s="1">
         <v>87</v>
       </c>
-      <c r="M78" s="73" t="str">
+      <c r="M78" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_articles &amp; " (" &amp; C$75 &amp; "," &amp; D$75 &amp; "," &amp; E$75 &amp; ") VALUES ('" &amp; C78 &amp; "','" &amp; D78 &amp; "','" &amp; E78 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_articles (article_id,warehouse_id,quantity) VALUES ('3','4','87')</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="E79" s="1">
         <v>23</v>
       </c>
-      <c r="M79" s="73" t="str">
+      <c r="M79" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_articles &amp; " (" &amp; C$75 &amp; "," &amp; D$75 &amp; "," &amp; E$75 &amp; ") VALUES ('" &amp; C79 &amp; "','" &amp; D79 &amp; "','" &amp; E79 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_articles (article_id,warehouse_id,quantity) VALUES ('4','5','23')</v>
       </c>
@@ -2920,17 +2920,17 @@
       <c r="E80" s="1">
         <v>45</v>
       </c>
-      <c r="M80" s="73" t="str">
+      <c r="M80" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_articles &amp; " (" &amp; C$75 &amp; "," &amp; D$75 &amp; "," &amp; E$75 &amp; ") VALUES ('" &amp; C80 &amp; "','" &amp; D80 &amp; "','" &amp; E80 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_articles (article_id,warehouse_id,quantity) VALUES ('5','5','45')</v>
       </c>
     </row>
     <row r="82" spans="2:13">
-      <c r="B82" s="70" t="s">
+      <c r="B82" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C82" s="71"/>
-      <c r="D82" s="72"/>
+      <c r="C82" s="73"/>
+      <c r="D82" s="74"/>
     </row>
     <row r="83" spans="2:13">
       <c r="B83" s="1" t="s">
@@ -2953,7 +2953,7 @@
       <c r="D84" s="31">
         <v>1</v>
       </c>
-      <c r="M84" s="73" t="str">
+      <c r="M84" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_employees &amp; " (" &amp; C$83 &amp; "," &amp; D$83 &amp; ") VALUES ('" &amp; C84 &amp; "','" &amp; D84 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_employees (warehouse_id,employees_id) VALUES ('1','1')</v>
       </c>
@@ -2968,7 +2968,7 @@
       <c r="D85" s="33">
         <v>2</v>
       </c>
-      <c r="M85" s="73" t="str">
+      <c r="M85" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_employees &amp; " (" &amp; C$83 &amp; "," &amp; D$83 &amp; ") VALUES ('" &amp; C85 &amp; "','" &amp; D85 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_employees (warehouse_id,employees_id) VALUES ('1','2')</v>
       </c>
@@ -2983,7 +2983,7 @@
       <c r="D86" s="32">
         <v>3</v>
       </c>
-      <c r="M86" s="73" t="str">
+      <c r="M86" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_employees &amp; " (" &amp; C$83 &amp; "," &amp; D$83 &amp; ") VALUES ('" &amp; C86 &amp; "','" &amp; D86 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_employees (warehouse_id,employees_id) VALUES ('1','3')</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="D87" s="34">
         <v>4</v>
       </c>
-      <c r="M87" s="73" t="str">
+      <c r="M87" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_employees &amp; " (" &amp; C$83 &amp; "," &amp; D$83 &amp; ") VALUES ('" &amp; C87 &amp; "','" &amp; D87 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_employees (warehouse_id,employees_id) VALUES ('3','4')</v>
       </c>
@@ -3013,19 +3013,19 @@
       <c r="D88" s="35">
         <v>5</v>
       </c>
-      <c r="M88" s="73" t="str">
+      <c r="M88" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_employees &amp; " (" &amp; C$83 &amp; "," &amp; D$83 &amp; ") VALUES ('" &amp; C88 &amp; "','" &amp; D88 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_employees (warehouse_id,employees_id) VALUES ('4','5')</v>
       </c>
     </row>
     <row r="90" spans="2:13">
-      <c r="B90" s="70" t="s">
+      <c r="B90" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C90" s="71"/>
-      <c r="D90" s="71"/>
-      <c r="E90" s="71"/>
-      <c r="F90" s="72"/>
+      <c r="C90" s="73"/>
+      <c r="D90" s="73"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="74"/>
     </row>
     <row r="91" spans="2:13">
       <c r="B91" s="1" t="s">
@@ -3060,7 +3060,7 @@
       <c r="F92" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="M92" s="73" t="str">
+      <c r="M92" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_days &amp; " (" &amp; C$91 &amp; "," &amp; D$91 &amp; "," &amp; F$91 &amp; "," &amp; F$91 &amp; ") VALUES ('" &amp; C92 &amp; "','" &amp; D92 &amp; "','" &amp; E92 &amp; "','" &amp; F92 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_days (warehouse_id,day_id,closingHours,closingHours) VALUES ('1','1',' 09:00','18:00')</v>
       </c>
@@ -3081,7 +3081,7 @@
       <c r="F93" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="M93" s="73" t="str">
+      <c r="M93" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_days &amp; " (" &amp; C$91 &amp; "," &amp; D$91 &amp; "," &amp; F$91 &amp; "," &amp; F$91 &amp; ") VALUES ('" &amp; C93 &amp; "','" &amp; D93 &amp; "','" &amp; E93 &amp; "','" &amp; F93 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_days (warehouse_id,day_id,closingHours,closingHours) VALUES ('2','2',' 08:30','17:30')</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="F94" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="M94" s="73" t="str">
+      <c r="M94" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_days &amp; " (" &amp; C$91 &amp; "," &amp; D$91 &amp; "," &amp; F$91 &amp; "," &amp; F$91 &amp; ") VALUES ('" &amp; C94 &amp; "','" &amp; D94 &amp; "','" &amp; E94 &amp; "','" &amp; F94 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_days (warehouse_id,day_id,closingHours,closingHours) VALUES ('3','3',' 10:00','19:00')</v>
       </c>
@@ -3123,7 +3123,7 @@
       <c r="F95" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="M95" s="73" t="str">
+      <c r="M95" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_days &amp; " (" &amp; C$91 &amp; "," &amp; D$91 &amp; "," &amp; F$91 &amp; "," &amp; F$91 &amp; ") VALUES ('" &amp; C95 &amp; "','" &amp; D95 &amp; "','" &amp; E95 &amp; "','" &amp; F95 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_days (warehouse_id,day_id,closingHours,closingHours) VALUES ('4','4',' 08:00','16:45')</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="F96" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="M96" s="73" t="str">
+      <c r="M96" s="70" t="str">
         <f>"INSERT INTO " &amp; warehouses_have_days &amp; " (" &amp; C$91 &amp; "," &amp; D$91 &amp; "," &amp; F$91 &amp; "," &amp; F$91 &amp; ") VALUES ('" &amp; C96 &amp; "','" &amp; D96 &amp; "','" &amp; E96 &amp; "','" &amp; F96 &amp; "')"</f>
         <v>INSERT INTO warehouses_have_days (warehouse_id,day_id,closingHours,closingHours) VALUES ('5','5',' 09:30','18:30')</v>
       </c>

</xml_diff>